<commit_message>
completed first step of new ppl
</commit_message>
<xml_diff>
--- a/2_code/list-sources.xlsx
+++ b/2_code/list-sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\consulting\projects\consulting\2_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E635DB77-0D3E-4689-856B-270D3215B7DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7039B8-1470-4E8B-BCC1-3468ACC3DCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A97FC25-B009-4150-BADE-91670A5B071B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A97FC25-B009-4150-BADE-91670A5B071B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>type</t>
   </si>
@@ -91,19 +91,31 @@
   </si>
   <si>
     <t>https://sites.google.com/view/germeval2017-absa/data?authuser=0</t>
+  </si>
+  <si>
+    <t>emoji-sentiment-ranking</t>
+  </si>
+  <si>
+    <t>https://www.clarin.si/repository/xmlui/handle/11356/1048</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,12 +134,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E34BDCA7-D9EE-4F93-8502-106E608DCE56}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -455,7 +485,7 @@
     <col min="3" max="3" width="75.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -466,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -477,7 +507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -488,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -499,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -510,7 +540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -521,7 +551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -532,7 +562,47 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D17" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>